<commit_message>
1. add fit_generator mode 2. add SequentialRandomChannelDataFeeder now we can training nn with financial data randomly extracted from raw data
</commit_message>
<xml_diff>
--- a/demo/tests_20180910.xlsx
+++ b/demo/tests_20180910.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="8820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="8820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="LorenzX" sheetId="2" r:id="rId2"/>
     <sheet name="Lorenz" sheetId="3" r:id="rId3"/>
     <sheet name="FinancialTop80volume" sheetId="4" r:id="rId4"/>
+    <sheet name="FinancialTop80volumeX6" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="123">
   <si>
     <t>1 layer stack</t>
   </si>
@@ -391,34 +392,83 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>0010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0100</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0200</t>
+  </si>
+  <si>
+    <t>0200</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0200</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>RUNNING</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0010</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0010</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0100</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0200</t>
-  </si>
-  <si>
-    <t>0200</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0200</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0010</t>
+    <t>RUNNING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>batches_per_epoch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>../data/prices.5min.top100volume/top80volumestocks.normalized.npy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>../model/FinancialTop80volumeX6/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0020</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G2.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G2.1lay.10ts.300hu.0200' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G3.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G3.1lay.100ts.100hu.0200' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G4.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G4.1lay.100ts.300hu.0200' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G5.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G5.5lay.10ts.100hu.0200' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G6.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G6.5lay.10ts.300hu.0200' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G7.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G7.5lay.100ts.100hu.0200' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G8.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G8.5lay.100ts.300hu.0200' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --test --test_length 500 --fit_generator --n_figs 10</t>
+  </si>
+  <si>
+    <t>screen -S FinData-CR-G1.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G1.1lay.10ts.100hu.0020' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --test --test_length 500 --fit_generator --n_figs 10</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -585,7 +635,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -612,6 +662,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -961,50 +1014,50 @@
   <sheetData>
     <row r="2" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="20" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="15" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="15" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="15" t="s">
+      <c r="L4" s="17"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="2:34" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1288,23 +1341,23 @@
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
-      <c r="AH14" s="18"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="19"/>
     </row>
     <row r="33" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
@@ -1450,15 +1503,15 @@
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1482,49 +1535,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9:AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
     </row>
     <row r="2" spans="1:35" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
@@ -1582,7 +1635,7 @@
       </c>
     </row>
     <row r="3" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1610,31 +1663,31 @@
         <v>10</v>
       </c>
       <c r="J3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="2">
         <v>64</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="19" t="str">
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:N10" si="0">CONCATENATE("screen -S ", B3, " python lstm.keras.py ", E3, " ", C3, " --data_path '", $L$3, "' --model_path '", $M$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu' --stages ", I3, " --epochs ", J3, " --batch_size ", K3," --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --data_scale")</f>
-        <v>screen -S LorenzX-CR-G1 python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G1.1lay.10ts.100hu' --stages 10 --epochs 1 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale</v>
-      </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
+        <v>screen -S LorenzX-CR-G1 python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G1.1lay.10ts.100hu' --stages 10 --epochs 2 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
       <c r="W3" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="X3">
         <v>10</v>
@@ -1642,24 +1695,24 @@
       <c r="Y3">
         <v>500</v>
       </c>
-      <c r="Z3" s="19" t="str">
+      <c r="Z3" s="20" t="str">
         <f t="shared" ref="Z3:Z10" si="1">CONCATENATE("screen -S ", B3, ".test python lstm.keras.py ", E3, " ", C3, " --data_path '", $L$3, "' --model_path '", $M$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu.", W3, "' --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --data_scale --test --test_length ", Y3, " --n_figs ", X3)</f>
-        <v>screen -S LorenzX-CR-G1.test python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G1.1lay.10ts.100hu.0010' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale --test --test_length 500 --n_figs 10</v>
-      </c>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
+        <v>screen -S LorenzX-CR-G1.test python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G1.1lay.10ts.100hu.0004' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale --test --test_length 500 --n_figs 10</v>
+      </c>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
       <c r="AI3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1690,20 +1743,20 @@
       <c r="K4">
         <v>64</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="19" t="str">
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G2 python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G2.1lay.10ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
       <c r="W4" s="8" t="s">
         <v>70</v>
       </c>
@@ -1713,24 +1766,24 @@
       <c r="Y4">
         <v>500</v>
       </c>
-      <c r="Z4" s="19" t="str">
+      <c r="Z4" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G2.test python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G2.1lay.10ts.300hu.0100' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="19"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
       <c r="AI4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1761,20 +1814,20 @@
       <c r="K5" s="2">
         <v>64</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="19" t="str">
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G3 python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G3.1lay.100ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
       <c r="W5" s="8" t="s">
         <v>69</v>
       </c>
@@ -1784,24 +1837,24 @@
       <c r="Y5">
         <v>500</v>
       </c>
-      <c r="Z5" s="19" t="str">
+      <c r="Z5" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G3.test python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G3.1lay.100ts.100hu.0100' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
       <c r="AI5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1832,20 +1885,20 @@
       <c r="K6">
         <v>64</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="19" t="str">
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G4 python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G4.1lay.100ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
       <c r="W6" s="8" t="s">
         <v>69</v>
       </c>
@@ -1855,24 +1908,24 @@
       <c r="Y6">
         <v>500</v>
       </c>
-      <c r="Z6" s="19" t="str">
+      <c r="Z6" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G4.test python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G4.1lay.100ts.300hu.0100' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
       <c r="AI6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1903,20 +1956,20 @@
       <c r="K7" s="2">
         <v>64</v>
       </c>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="19" t="str">
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G5 python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G5.5lay.10ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
       <c r="W7" s="8" t="s">
         <v>99</v>
       </c>
@@ -1926,24 +1979,24 @@
       <c r="Y7">
         <v>500</v>
       </c>
-      <c r="Z7" s="19" t="str">
+      <c r="Z7" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G5.test python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G5.5lay.10ts.100hu.0050' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-      <c r="AH7" s="19"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
       <c r="AI7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1974,20 +2027,20 @@
       <c r="K8">
         <v>64</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="19" t="str">
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G6 python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G6.5lay.10ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
       <c r="W8" s="8" t="s">
         <v>100</v>
       </c>
@@ -1997,24 +2050,24 @@
       <c r="Y8">
         <v>500</v>
       </c>
-      <c r="Z8" s="19" t="str">
+      <c r="Z8" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G6.test python lstm.keras.py 10 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G6.5lay.10ts.300hu.0070' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="19"/>
-      <c r="AG8" s="19"/>
-      <c r="AH8" s="19"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
       <c r="AI8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2045,22 +2098,22 @@
       <c r="K9" s="2">
         <v>64</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="19" t="str">
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G7 python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G7.5lay.100ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
       <c r="W9" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="X9">
         <v>10</v>
@@ -2068,24 +2121,24 @@
       <c r="Y9">
         <v>500</v>
       </c>
-      <c r="Z9" s="19" t="str">
+      <c r="Z9" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G7.test python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G7.5lay.100ts.100hu.0010' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="19"/>
-      <c r="AH9" s="19"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
       <c r="AI9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2116,22 +2169,22 @@
       <c r="K10">
         <v>64</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="19" t="str">
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S LorenzX-CR-G8 python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G8.5lay.100ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
       <c r="W10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X10">
         <v>10</v>
@@ -2139,177 +2192,177 @@
       <c r="Y10">
         <v>500</v>
       </c>
-      <c r="Z10" s="19" t="str">
+      <c r="Z10" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S LorenzX-CR-G8.test python lstm.keras.py 100 1 --data_path '../data/Lorenz_1_100000_x.npy' --model_path '../model/LorenzX/LorenzX-CR-G8.5lay.100ts.300hu.0010' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
-      <c r="AH10" s="19"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
       <c r="AI10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
+      <c r="A11" s="22"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
     </row>
     <row r="12" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
     </row>
     <row r="13" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
     </row>
     <row r="14" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
     </row>
     <row r="15" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
     </row>
     <row r="16" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="19"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
     </row>
     <row r="17" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
     </row>
     <row r="18" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
     </row>
     <row r="19" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -2355,7 +2408,7 @@
   <dimension ref="A1:AI19"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="AI9" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2364,42 +2417,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
     </row>
     <row r="2" spans="1:35" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
@@ -2457,7 +2510,7 @@
       </c>
     </row>
     <row r="3" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2490,24 +2543,24 @@
       <c r="K3" s="2">
         <v>64</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="19" t="str">
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:N10" si="0">CONCATENATE("screen -S ", B3, " python lstm.keras.py ", E3, " ", C3, " --data_path '", $L$3, "' --model_path '", $M$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu' --stages ", I3, " --epochs ", J3, " --batch_size ", K3," --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --data_scale")</f>
         <v>screen -S Lorenz-CR-G1 python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G1.1lay.10ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
       <c r="W3" s="8" t="s">
         <v>68</v>
       </c>
@@ -2517,24 +2570,24 @@
       <c r="Y3">
         <v>500</v>
       </c>
-      <c r="Z3" s="19" t="str">
+      <c r="Z3" s="20" t="str">
         <f t="shared" ref="Z3:Z10" si="1">CONCATENATE("screen -S ", B3, ".test python lstm.keras.py ", E3, " ", C3, " --data_path '", $L$3, "' --model_path '", $M$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu.", W3, "' --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --data_scale --test --test_length ", Y3, " --n_figs ", X3)</f>
         <v>screen -S Lorenz-CR-G1.test python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G1.1lay.10ts.100hu.0100' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
       <c r="AI3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
@@ -2565,20 +2618,20 @@
       <c r="K4">
         <v>64</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="19" t="str">
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G2 python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G2.1lay.10ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
       <c r="W4" s="8" t="s">
         <v>70</v>
       </c>
@@ -2588,24 +2641,24 @@
       <c r="Y4">
         <v>500</v>
       </c>
-      <c r="Z4" s="19" t="str">
+      <c r="Z4" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G2.test python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G2.1lay.10ts.300hu.0100' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="19"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
       <c r="AI4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
@@ -2636,20 +2689,20 @@
       <c r="K5" s="2">
         <v>64</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="19" t="str">
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G3 python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G3.1lay.100ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
       <c r="W5" s="8" t="s">
         <v>69</v>
       </c>
@@ -2659,24 +2712,24 @@
       <c r="Y5">
         <v>500</v>
       </c>
-      <c r="Z5" s="19" t="str">
+      <c r="Z5" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G3.test python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G3.1lay.100ts.100hu.0100' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
       <c r="AI5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="1" t="s">
         <v>82</v>
       </c>
@@ -2707,20 +2760,20 @@
       <c r="K6">
         <v>64</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="19" t="str">
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G4 python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G4.1lay.100ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
       <c r="W6" s="8" t="s">
         <v>69</v>
       </c>
@@ -2730,24 +2783,24 @@
       <c r="Y6">
         <v>500</v>
       </c>
-      <c r="Z6" s="19" t="str">
+      <c r="Z6" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G4.test python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G4.1lay.100ts.300hu.0100' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
       <c r="AI6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
         <v>83</v>
       </c>
@@ -2778,22 +2831,22 @@
       <c r="K7" s="2">
         <v>64</v>
       </c>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="19" t="str">
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G5 python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G5.5lay.10ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
       <c r="W7" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X7">
         <v>10</v>
@@ -2801,24 +2854,24 @@
       <c r="Y7">
         <v>500</v>
       </c>
-      <c r="Z7" s="19" t="str">
+      <c r="Z7" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G5.test python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G5.5lay.10ts.100hu.0100' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-      <c r="AH7" s="19"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
       <c r="AI7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>84</v>
       </c>
@@ -2849,20 +2902,20 @@
       <c r="K8">
         <v>64</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="19" t="str">
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G6 python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G6.5lay.10ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
       <c r="W8" s="8" t="s">
         <v>69</v>
       </c>
@@ -2872,24 +2925,24 @@
       <c r="Y8">
         <v>500</v>
       </c>
-      <c r="Z8" s="19" t="str">
+      <c r="Z8" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G6.test python lstm.keras.py 10 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G6.5lay.10ts.300hu.0100' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="19"/>
-      <c r="AG8" s="19"/>
-      <c r="AH8" s="19"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
       <c r="AI8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="1" t="s">
         <v>85</v>
       </c>
@@ -2920,20 +2973,20 @@
       <c r="K9" s="2">
         <v>64</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="19" t="str">
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G7 python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G7.5lay.100ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale</v>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
       <c r="W9" s="8" t="s">
         <v>69</v>
       </c>
@@ -2943,21 +2996,21 @@
       <c r="Y9">
         <v>500</v>
       </c>
-      <c r="Z9" s="19" t="str">
+      <c r="Z9" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G7.test python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G7.5lay.100ts.100hu.0100' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="19"/>
-      <c r="AH9" s="19"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
     </row>
     <row r="10" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
         <v>86</v>
       </c>
@@ -2988,20 +3041,20 @@
       <c r="K10">
         <v>64</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="19" t="str">
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S Lorenz-CR-G8 python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G8.5lay.100ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
       <c r="W10" s="8" t="s">
         <v>69</v>
       </c>
@@ -3011,174 +3064,174 @@
       <c r="Y10">
         <v>500</v>
       </c>
-      <c r="Z10" s="19" t="str">
+      <c r="Z10" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S Lorenz-CR-G8.test python lstm.keras.py 100 3 --data_path '../data/Lorenz_1_100000.npy' --model_path '../model/Lorenz/Lorenz-CR-G8.5lay.100ts.300hu.0100' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
-      <c r="AH10" s="19"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
     </row>
     <row r="11" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
+      <c r="A11" s="22"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
     </row>
     <row r="12" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
     </row>
     <row r="13" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
     </row>
     <row r="14" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
     </row>
     <row r="15" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
     </row>
     <row r="16" spans="1:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="19"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
     </row>
     <row r="17" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
     </row>
     <row r="18" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
     </row>
     <row r="19" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -3223,8 +3276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI19"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6:AH6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3233,42 +3286,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
     </row>
     <row r="2" spans="2:35" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
@@ -3356,26 +3409,26 @@
       <c r="K3" s="2">
         <v>64</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="19" t="str">
+      <c r="N3" s="20" t="str">
         <f t="shared" ref="N3:N10" si="0">CONCATENATE("screen -S ", B3, " python lstm.keras.py ", E3, " ", C3, " --data_path '", $L$3, "' --model_path '", $M$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu' --stages ", I3, " --epochs ", J3, " --batch_size ", K3," --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --data_scale")</f>
         <v>screen -S FinData-CR-G1 python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G1.1lay.10ts.100hu' --stages 20 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
       <c r="W3" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="X3">
         <v>10</v>
@@ -3383,20 +3436,20 @@
       <c r="Y3">
         <v>500</v>
       </c>
-      <c r="Z3" s="19" t="str">
+      <c r="Z3" s="20" t="str">
         <f t="shared" ref="Z3:Z10" si="1">CONCATENATE("screen -S ", B3, ".test python lstm.keras.py ", E3, " ", C3, " --data_path '", $L$3, "' --model_path '", $M$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu.", W3, "' --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --data_scale --test --test_length ", Y3, " --n_figs ", X3)</f>
         <v>screen -S FinData-CR-G1.test python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G1.1lay.10ts.100hu.0200' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
       <c r="AI3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3430,22 +3483,22 @@
       <c r="K4">
         <v>64</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="19" t="str">
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G2 python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G2.1lay.10ts.300hu' --stages 20 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
       <c r="W4" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="X4">
         <v>10</v>
@@ -3453,20 +3506,20 @@
       <c r="Y4">
         <v>500</v>
       </c>
-      <c r="Z4" s="19" t="str">
+      <c r="Z4" s="20" t="str">
         <f>CONCATENATE("screen -S ", B4, ".test python lstm.keras.py ", E4, " ", C4, " --data_path '", $L$3, "' --model_path '", $M$3, B4, ".", D4, "lay", ".", E4, "ts.", F4, "hu.", W4, "' --Solver ", G4, " --hidden_units ", F4, " --CUDA_VISIBLE_DEVICES ", H4, " --data_scale --test --test_length ", Y4, " --n_figs ", X4)</f>
         <v>screen -S FinData-CR-G2.test python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G2.1lay.10ts.300hu.0200' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="19"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
       <c r="AI4" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3500,22 +3553,22 @@
       <c r="K5" s="2">
         <v>64</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="19" t="str">
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G3 python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G3.1lay.100ts.100hu' --stages 20 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
       <c r="W5" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X5">
         <v>10</v>
@@ -3523,20 +3576,20 @@
       <c r="Y5">
         <v>500</v>
       </c>
-      <c r="Z5" s="19" t="str">
+      <c r="Z5" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S FinData-CR-G3.test python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G3.1lay.100ts.100hu.0200' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
       <c r="AI5" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3570,22 +3623,22 @@
       <c r="K6">
         <v>64</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="19" t="str">
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G4 python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G4.1lay.100ts.300hu' --stages 20 --epochs 10 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
       <c r="W6" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X6">
         <v>10</v>
@@ -3593,20 +3646,20 @@
       <c r="Y6">
         <v>500</v>
       </c>
-      <c r="Z6" s="19" t="str">
+      <c r="Z6" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S FinData-CR-G4.test python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G4.1lay.100ts.300hu.0200' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
       <c r="AI6" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3640,22 +3693,22 @@
       <c r="K7" s="2">
         <v>64</v>
       </c>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="19" t="str">
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G5 python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G5.5lay.10ts.100hu' --stages 20 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
       <c r="W7" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X7">
         <v>10</v>
@@ -3663,18 +3716,21 @@
       <c r="Y7">
         <v>500</v>
       </c>
-      <c r="Z7" s="19" t="str">
+      <c r="Z7" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S FinData-CR-G5.test python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G5.5lay.10ts.100hu.0200' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-      <c r="AH7" s="19"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="8" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -3707,22 +3763,22 @@
       <c r="K8">
         <v>64</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="19" t="str">
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G6 python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G6.5lay.10ts.300hu' --stages 20 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
       <c r="W8" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X8">
         <v>10</v>
@@ -3730,18 +3786,21 @@
       <c r="Y8">
         <v>500</v>
       </c>
-      <c r="Z8" s="19" t="str">
+      <c r="Z8" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S FinData-CR-G6.test python lstm.keras.py 10 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G6.5lay.10ts.300hu.0200' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="19"/>
-      <c r="AG8" s="19"/>
-      <c r="AH8" s="19"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -3774,22 +3833,22 @@
       <c r="K9" s="2">
         <v>64</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="19" t="str">
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G7 python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G7.5lay.100ts.100hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale</v>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
       <c r="W9" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X9">
         <v>10</v>
@@ -3797,18 +3856,18 @@
       <c r="Y9">
         <v>500</v>
       </c>
-      <c r="Z9" s="19" t="str">
+      <c r="Z9" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S FinData-CR-G7.test python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G7.5lay.100ts.100hu.0200' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="19"/>
-      <c r="AH9" s="19"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
     </row>
     <row r="10" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -3841,22 +3900,22 @@
       <c r="K10">
         <v>64</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="19" t="str">
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>screen -S FinData-CR-G8 python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G8.5lay.100ts.300hu' --stages 10 --epochs 10 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale</v>
       </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
       <c r="W10" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X10">
         <v>10</v>
@@ -3864,131 +3923,131 @@
       <c r="Y10">
         <v>500</v>
       </c>
-      <c r="Z10" s="19" t="str">
+      <c r="Z10" s="20" t="str">
         <f t="shared" si="1"/>
         <v>screen -S FinData-CR-G8.test python lstm.keras.py 100 80 --data_path '../data/prices.5min.top100volume/top80volumestocks.csv' --model_path '../model/FinancialTop80volume/FinData-CR-G8.5lay.100ts.300hu.0200' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --data_scale --test --test_length 500 --n_figs 10</v>
       </c>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
-      <c r="AH10" s="19"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
     </row>
     <row r="11" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
     </row>
     <row r="13" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
     </row>
     <row r="14" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
     </row>
     <row r="15" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
     </row>
     <row r="16" spans="2:35" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
-      <c r="V16" s="19"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
     </row>
     <row r="17" spans="2:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
     </row>
     <row r="18" spans="2:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
     </row>
     <row r="19" spans="2:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -4024,4 +4083,869 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AK19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AK10" sqref="AK10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="C1" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+    </row>
+    <row r="2" spans="2:37" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="X2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2">
+        <v>64</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" s="20" t="str">
+        <f>CONCATENATE("screen -S ", B3, " python lstm.keras.v2.py ", E3, " ", C3, " --data_path '", $M$3, "' --model_path '", $N$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu' --stages ", I3, " --epochs ", J3, " --batches_per_epoch ", L3, " --batch_size ", K3, " --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --fit_generator")</f>
+        <v>screen -S FinData-CR-G1 python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G1.1lay.10ts.100hu' --stages 20 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --fit_generator</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y3">
+        <v>10</v>
+      </c>
+      <c r="Z3">
+        <v>500</v>
+      </c>
+      <c r="AA3" s="20" t="str">
+        <f>CONCATENATE("screen -S ", B3, ".test python lstm.keras.v2.py ", E3, " ", C3, " --data_path '", $M$3, "' --model_path '", $N$3, B3, ".", D3, "lay", ".", E3, "ts.", F3, "hu.", X3, "' --Solver ", G3, " --hidden_units ", F3, " --CUDA_VISIBLE_DEVICES ", H3, " --test --test_length ", Z3, " --fit_generator --n_figs ", Y3)</f>
+        <v>screen -S FinData-CR-G1.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G1.1lay.10ts.100hu.0020' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>300</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>64</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="20" t="str">
+        <f t="shared" ref="O4:O10" si="0">CONCATENATE("screen -S ", B4, " python lstm.keras.v2.py ", E4, " ", C4, " --data_path '", $M$3, "' --model_path '", $N$3, B4, ".", D4, "lay", ".", E4, "ts.", F4, "hu' --stages ", I4, " --epochs ", J4, " --batches_per_epoch ", L4, " --batch_size ", K4, " --Solver ", G4, " --hidden_units ", F4, " --CUDA_VISIBLE_DEVICES ", H4, " --fit_generator")</f>
+        <v>screen -S FinData-CR-G2 python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G2.1lay.10ts.300hu' --stages 20 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --fit_generator</v>
+      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y4">
+        <v>10</v>
+      </c>
+      <c r="Z4">
+        <v>500</v>
+      </c>
+      <c r="AA4" s="20" t="str">
+        <f t="shared" ref="AA4:AA10" si="1">CONCATENATE("screen -S ", B4, ".test python lstm.keras.v2.py ", E4, " ", C4, " --data_path '", $M$3, "' --model_path '", $N$3, B4, ".", D4, "lay", ".", E4, "ts.", F4, "hu.", X4, "' --Solver ", G4, " --hidden_units ", F4, " --CUDA_VISIBLE_DEVICES ", H4, " --test --test_length ", Z4, " --fit_generator --n_figs ", Y4)</f>
+        <v>screen -S FinData-CR-G2.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G2.1lay.10ts.300hu.0200' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2">
+        <v>64</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>screen -S FinData-CR-G3 python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G3.1lay.100ts.100hu' --stages 20 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --fit_generator</v>
+      </c>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y5">
+        <v>10</v>
+      </c>
+      <c r="Z5">
+        <v>500</v>
+      </c>
+      <c r="AA5" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>screen -S FinData-CR-G3.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G3.1lay.100ts.100hu.0200' --Solver SolverStructure2 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>64</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>screen -S FinData-CR-G4 python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G4.1lay.100ts.300hu' --stages 20 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --fit_generator</v>
+      </c>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6">
+        <v>500</v>
+      </c>
+      <c r="AA6" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>screen -S FinData-CR-G4.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G4.1lay.100ts.300hu.0200' --Solver SolverStructure2 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2">
+        <v>10</v>
+      </c>
+      <c r="K7" s="2">
+        <v>64</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>screen -S FinData-CR-G5 python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G5.5lay.10ts.100hu' --stages 20 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --fit_generator</v>
+      </c>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y7">
+        <v>10</v>
+      </c>
+      <c r="Z7">
+        <v>500</v>
+      </c>
+      <c r="AA7" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>screen -S FinData-CR-G5.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G5.5lay.10ts.100hu.0200' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 0 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>64</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>screen -S FinData-CR-G6 python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G6.5lay.10ts.300hu' --stages 20 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --fit_generator</v>
+      </c>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y8">
+        <v>10</v>
+      </c>
+      <c r="Z8">
+        <v>500</v>
+      </c>
+      <c r="AA8" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>screen -S FinData-CR-G6.test python lstm.keras.v2.py 10 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G6.5lay.10ts.300hu.0200' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 1 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AJ8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>10</v>
+      </c>
+      <c r="J9" s="2">
+        <v>10</v>
+      </c>
+      <c r="K9" s="2">
+        <v>64</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>screen -S FinData-CR-G7 python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G7.5lay.100ts.100hu' --stages 10 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --fit_generator</v>
+      </c>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y9">
+        <v>10</v>
+      </c>
+      <c r="Z9">
+        <v>500</v>
+      </c>
+      <c r="AA9" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>screen -S FinData-CR-G7.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G7.5lay.100ts.100hu.0200' --Solver SolverStructure3 --hidden_units 100 --CUDA_VISIBLE_DEVICES 2 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20"/>
+      <c r="AK9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>300</v>
+      </c>
+      <c r="G10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>64</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>screen -S FinData-CR-G8 python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G8.5lay.100ts.300hu' --stages 10 --epochs 10 --batches_per_epoch 1000 --batch_size 64 --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --fit_generator</v>
+      </c>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y10">
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <v>500</v>
+      </c>
+      <c r="AA10" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>screen -S FinData-CR-G8.test python lstm.keras.v2.py 100 6 --data_path '../data/prices.5min.top100volume/top80volumestocks.normalized.npy' --model_path '../model/FinancialTop80volumeX6/FinData-CR-G8.5lay.100ts.300hu.0200' --Solver SolverStructure3 --hidden_units 300 --CUDA_VISIBLE_DEVICES 3 --test --test_length 500 --fit_generator --n_figs 10</v>
+      </c>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AK10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+    </row>
+    <row r="13" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+    </row>
+    <row r="14" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+    </row>
+    <row r="15" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+    </row>
+    <row r="16" spans="2:37" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+    </row>
+    <row r="17" spans="2:23" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+    </row>
+    <row r="18" spans="2:23" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+    </row>
+    <row r="19" spans="2:23" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="AA4:AI4"/>
+    <mergeCell ref="O14:W14"/>
+    <mergeCell ref="O15:W15"/>
+    <mergeCell ref="O16:W16"/>
+    <mergeCell ref="O17:W17"/>
+    <mergeCell ref="O18:W18"/>
+    <mergeCell ref="O19:W19"/>
+    <mergeCell ref="O9:W9"/>
+    <mergeCell ref="AA9:AI9"/>
+    <mergeCell ref="O10:W10"/>
+    <mergeCell ref="AA10:AI10"/>
+    <mergeCell ref="O12:W12"/>
+    <mergeCell ref="O13:W13"/>
+    <mergeCell ref="O6:W6"/>
+    <mergeCell ref="AA6:AI6"/>
+    <mergeCell ref="O7:W7"/>
+    <mergeCell ref="AA7:AI7"/>
+    <mergeCell ref="O8:W8"/>
+    <mergeCell ref="AA8:AI8"/>
+    <mergeCell ref="C1:W1"/>
+    <mergeCell ref="X1:AI1"/>
+    <mergeCell ref="M3:M10"/>
+    <mergeCell ref="N3:N10"/>
+    <mergeCell ref="O3:W3"/>
+    <mergeCell ref="O4:W4"/>
+    <mergeCell ref="AA3:AI3"/>
+    <mergeCell ref="O5:W5"/>
+    <mergeCell ref="AA5:AI5"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>